<commit_message>
java data clean and time update
</commit_message>
<xml_diff>
--- a/DataCleanValidation/bin/validation/test/GraphStructure.xlsx
+++ b/DataCleanValidation/bin/validation/test/GraphStructure.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="17235" windowHeight="8250"/>
+    <workbookView xWindow="0" yWindow="2820" windowWidth="13635" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="graph" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -408,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>